<commit_message>
Test Suite punctuation cases.
</commit_message>
<xml_diff>
--- a/doc/Sentences_Checklist_0.1.xlsx
+++ b/doc/Sentences_Checklist_0.1.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
   <si>
     <t>Sentence</t>
   </si>
@@ -123,6 +123,18 @@
   </si>
   <si>
     <t>Every word</t>
+  </si>
+  <si>
+    <t>Same word</t>
+  </si>
+  <si>
+    <t>Duplicate longest word returned only once.</t>
+  </si>
+  <si>
+    <t>Same word, different case</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
@@ -487,7 +499,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M87"/>
+  <dimension ref="A1:M89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -533,7 +545,7 @@
         <v>17</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -541,7 +553,7 @@
         <v>5</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -557,7 +569,7 @@
         <v>18</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -617,24 +629,30 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B15" s="1" t="s">
+      <c r="D15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C17" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>30</v>
@@ -642,15 +660,15 @@
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C18" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="D19" s="1" t="s">
-        <v>16</v>
+      <c r="C19" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>30</v>
@@ -658,7 +676,7 @@
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C20" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>30</v>
@@ -666,23 +684,23 @@
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="D21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D23" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="D22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C23" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>30</v>
@@ -690,55 +708,55 @@
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.3">
       <c r="D24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D26" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K24" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="D25" s="1" t="s">
+      <c r="K26" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D27" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K25" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C26" s="1" t="s">
+      <c r="K27" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C28" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K26" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B27" s="1" t="s">
+      <c r="K28" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K27" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B28" s="1" t="s">
+      <c r="K29" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B30" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C29" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C30" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>30</v>
@@ -746,14 +764,30 @@
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C31" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C32" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C33" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K31" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="87" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E87" s="2"/>
+      <c r="K33" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="89" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E89" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>